<commit_message>
Theme updated according to warning class of bootstrap.
</commit_message>
<xml_diff>
--- a/Project Summary.xlsx
+++ b/Project Summary.xlsx
@@ -237,15 +237,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,14 +539,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -593,7 +593,7 @@
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4"/>
@@ -659,52 +659,52 @@
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Booking and reservation done.
</commit_message>
<xml_diff>
--- a/Project Summary.xlsx
+++ b/Project Summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Status</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>• Cost-effective.</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <dimension ref="B2:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,13 +563,17 @@
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">

</xml_diff>

<commit_message>
Cancel request functionality done.
</commit_message>
<xml_diff>
--- a/Project Summary.xlsx
+++ b/Project Summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Status</t>
   </si>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,9 @@
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -591,37 +593,49 @@
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
@@ -633,7 +647,9 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
@@ -645,7 +661,9 @@
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
@@ -689,21 +707,33 @@
       <c r="B26" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="C26" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="C27" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="C28" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
         <v>25</v>
       </c>
+      <c r="C29" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
@@ -713,6 +743,9 @@
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
         <v>27</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>